<commit_message>
Updated photos and some bios
</commit_message>
<xml_diff>
--- a/src/data/winter23/bios_winter23.xlsx
+++ b/src/data/winter23/bios_winter23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\winter23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A24F3A-2C36-4DB0-BC26-786B51E6AED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A25C18-B248-43F4-B9C7-882CB0286D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="690" windowWidth="25680" windowHeight="14910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="507">
   <si>
     <t>Timestamp</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Finance, Consulting</t>
   </si>
   <si>
-    <t>Finance Intern at Facebook</t>
-  </si>
-  <si>
     <t>UFA, Tri Delta</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t>Private Equity, Consulting, Finance</t>
   </si>
   <si>
-    <t>Private Equity Summer Analyst at The Everstone Group</t>
-  </si>
-  <si>
     <t>SCNO, MAISS, UCI Esports, Quokka Brew Ambassadors</t>
   </si>
   <si>
@@ -409,9 +403,6 @@
     <t>Sales and Trading</t>
   </si>
   <si>
-    <t>Private Equity Investment Intern at Pathway Capital Management</t>
-  </si>
-  <si>
     <t>Undergraduate Finance Association, Student-Managed Investment Fund, Irvine Banking Society</t>
   </si>
   <si>
@@ -469,9 +460,6 @@
     <t>Investment Banking</t>
   </si>
   <si>
-    <t>Investment Banking Summer Analyst at Deutsche Bank</t>
-  </si>
-  <si>
     <t>Jenny</t>
   </si>
   <si>
@@ -520,9 +508,6 @@
     <t>julie_luu</t>
   </si>
   <si>
-    <t>Business Strategy &amp; Marketing Intern at Autodesk</t>
-  </si>
-  <si>
     <t>ASUCI Marketing Strategy Intern ('21-22), MUSA VP of Communications ('20-21), MUSA Representative ('19-20)</t>
   </si>
   <si>
@@ -556,12 +541,6 @@
     <t>kevin_cao</t>
   </si>
   <si>
-    <t>Consulting, Software Engineering</t>
-  </si>
-  <si>
-    <t>Social Media Manager Intern at OPTIS Group Holdings</t>
-  </si>
-  <si>
     <t>ASUCI, MUSA, SCNO</t>
   </si>
   <si>
@@ -589,9 +568,6 @@
     <t>Product Marketing</t>
   </si>
   <si>
-    <t>Founder at A Drop of Delight</t>
-  </si>
-  <si>
     <t>MAISS, Hack at UCI, UCI Alumni Association</t>
   </si>
   <si>
@@ -616,9 +592,6 @@
     <t>SuZhou, China; Temple City, CA</t>
   </si>
   <si>
-    <t>Portfolio Analyst Intern at Wells Fargo Advisors</t>
-  </si>
-  <si>
     <t>Undergraduate Finance Association, Undergraduate Business Association</t>
   </si>
   <si>
@@ -629,9 +602,6 @@
   </si>
   <si>
     <t>Real Estate</t>
-  </si>
-  <si>
-    <t>Acquisition Analyst at Next Wave Investors</t>
   </si>
   <si>
     <t>Irvine Banking Society</t>
@@ -695,9 +665,6 @@
     <t>Consulting, Finance</t>
   </si>
   <si>
-    <t xml:space="preserve">Summer Research Consulting Intern at Linda S. Congleton &amp; Associates </t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/tommytruong482/</t>
   </si>
   <si>
@@ -722,9 +689,6 @@
     <t>yeseohan@ucidsp.com</t>
   </si>
   <si>
-    <t>Social Media Intern at J.ING</t>
-  </si>
-  <si>
     <t>Nathan</t>
   </si>
   <si>
@@ -764,9 +728,6 @@
     <t>Consulting, Investing</t>
   </si>
   <si>
-    <t>Risk and Financial Advisory Intern at Deloitte</t>
-  </si>
-  <si>
     <t>Dragon Boat Race Team</t>
   </si>
   <si>
@@ -788,9 +749,6 @@
     <t>Basking Ridge, NJ</t>
   </si>
   <si>
-    <t>Investment Banking, Finance, Esports</t>
-  </si>
-  <si>
     <t>foresthuang@ucidsp.com</t>
   </si>
   <si>
@@ -809,9 +767,6 @@
     <t>Portland, OR</t>
   </si>
   <si>
-    <t>MUSA Representatives</t>
-  </si>
-  <si>
     <t>julialin@ucidsp.com</t>
   </si>
   <si>
@@ -920,12 +875,6 @@
     <t>andrewdoan@ucidsp.com</t>
   </si>
   <si>
-    <t>Product Association, ASUCI</t>
-  </si>
-  <si>
-    <t>Partner at California Crescent Fund</t>
-  </si>
-  <si>
     <t>Anthropology, Digital Information Systems</t>
   </si>
   <si>
@@ -941,9 +890,6 @@
     <t>My name is Grace and I initiated fall my freshman year with the Alpha Iotas! I'm extremely stoked to meet all of you :) Ask me about my favorite books, work life balance, rollerskating, night life in NY, travel, makeup and fashion! Reach out with any questions, would love to chat!</t>
   </si>
   <si>
-    <t>Venture Capital and Business Analytic Extern at HP Tech Ventures</t>
-  </si>
-  <si>
     <t>Real Estate Association, Sigma Chi, RUF</t>
   </si>
   <si>
@@ -953,12 +899,6 @@
     <t>Hi! My name is Dylan, and I initiated in the spring quarter of my first year. In my free time, I enjoy playing volleyball, basketball, and Valorant. Feel free to ask me about cars, options trading, and random stuff. Looking forward to seeing you :)</t>
   </si>
   <si>
-    <t>Intern at Linda S. Congleton &amp; Associates</t>
-  </si>
-  <si>
-    <t>Incoming Educator at Lululemon</t>
-  </si>
-  <si>
     <t>Sports Business Association</t>
   </si>
   <si>
@@ -968,12 +908,6 @@
     <t>Product Design, Product Management</t>
   </si>
   <si>
-    <t>UCI Athletics Marketing Intern</t>
-  </si>
-  <si>
-    <t>Product Design Lead at Product Association</t>
-  </si>
-  <si>
     <t>Jorina</t>
   </si>
   <si>
@@ -986,12 +920,6 @@
     <t>Alpha Nu</t>
   </si>
   <si>
-    <t>Innovation and Entrepreneurship</t>
-  </si>
-  <si>
-    <t>UX Research Intern at Zendesk</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/jorinachen</t>
   </si>
   <si>
@@ -1019,9 +947,6 @@
     <t>Accounting, Finance</t>
   </si>
   <si>
-    <t>Accounting Project Associate at First Foundation Bank</t>
-  </si>
-  <si>
     <t>Hi!! My name is Haley and I initiated in the spring of my sophomore year with the Alpha Nu class. In my free time, I enjoy swimming, reading, trying new food/boba places, and taking film photos. Feel free to ask me about my boba blog, favorite books, or anything else at recruitment!</t>
   </si>
   <si>
@@ -1064,24 +989,12 @@
     <t>aryan_bajaria</t>
   </si>
   <si>
-    <t>Real Estate, Consulting, Venture Capital</t>
-  </si>
-  <si>
-    <t>Keller Williams Realty Firm</t>
-  </si>
-  <si>
-    <t>REA, Mesa Court Housing, Sigma Chi</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/aryanbajaria/</t>
   </si>
   <si>
     <t>aryanbajaria@ucidsp.com</t>
   </si>
   <si>
-    <t>Hello! My name is Aryan, and I initiated spring quarter of my freshman year with the Alpha Nu class! In my free time, you will find me exploring nature, staying active at the gym, playing soccer, or exploring new areas. A fun fact about me is that I stuck my finger in a blender when I was a kid. Ask me about Formula 1 or my passion for cars at recruitment, I look forward to meeting you!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Madeline </t>
   </si>
   <si>
@@ -1103,21 +1016,12 @@
     <t>Film and Media Studies</t>
   </si>
   <si>
-    <t>Marketing, Public Relations, Consulting</t>
-  </si>
-  <si>
-    <t>UUMP</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/madeline-li-b4959a1a5/</t>
   </si>
   <si>
     <t>madelineli@ucidsp.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi! My name is Maddie and I initiated the spring quarter of my second year with the Alpha Nu class. In my free time, you can find me at the ARC playing volleyball or watching tv/movies. Feel free to ask me about my favorite animal or my 150+ Spotify playlists at recruitment! </t>
-  </si>
-  <si>
     <t xml:space="preserve">Jin </t>
   </si>
   <si>
@@ -1160,9 +1064,6 @@
     <t>Marketing, HR</t>
   </si>
   <si>
-    <t>Marketing Intern for KUCI 88.9 FM</t>
-  </si>
-  <si>
     <t>MUSA, Marketing Association, Art History Undergraduate Association, Model UN, KUCI 88.9 FM</t>
   </si>
   <si>
@@ -1202,54 +1103,30 @@
     <t>Domestic Media Marketing Intern @ Paramount Pictures Brand Development</t>
   </si>
   <si>
-    <t>Innovation and Entrepreneurship, Sociology</t>
-  </si>
-  <si>
     <t>Hey there! My name is Andrew and I initiated in Fall 2021 with the Alpha Mus. Professionally, I'm super interested in all things product, especially design! Beyond that, I love dance, art, poetry, music festivals, traveling, and good company. Looking forward to meeting you at recruitment :)</t>
   </si>
   <si>
-    <t>Software Developer at LinQuest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance/Business Operations Acquisition Intern at NASA Jet Propulsion Laboratory </t>
-  </si>
-  <si>
     <t>Amazon Prime Campus Ambassador, Campus Representatives, Red Bull Student Marketeer</t>
   </si>
   <si>
     <t>Hi! My name is Julia and I initiated in the fall of my freshman year with the Alpha Mu class. Some fun facts about me are that I’m a little bit of a shopaholic and that you might see me around campus giving tours since I’m a tour guide for UCI. Ask me about my favorite flavor of Red Bull or anything at recruitment :-)</t>
   </si>
   <si>
-    <t>Change Management Operations Intern at PayPal</t>
-  </si>
-  <si>
     <t xml:space="preserve">HRMA, Student Assistant at Paul Merage Specialty Masters Program, MUSA Representative </t>
   </si>
   <si>
-    <t>HR Intern at Kaiser Permanente</t>
-  </si>
-  <si>
-    <t>Finance Extern at Apple; Client Group Intern at Wellington</t>
-  </si>
-  <si>
     <t>Hi!! My name is Winnie and I initiated fall quarter of my second year with the Alpha Mu class. In my free time, I love playing basketball, trying new food spots, hammocking in Aldrich, and binge-watching architectural digest vids! Fun fact I've made 218+ Spotify playlists over the years! See you at recruitment :)</t>
   </si>
   <si>
     <t>Software Engineering, Finance</t>
   </si>
   <si>
-    <t>Software Engineering Intern at Duck Creek Technologies</t>
-  </si>
-  <si>
     <t>Association for Computing Machinery</t>
   </si>
   <si>
     <t>Public Health &amp; Management</t>
   </si>
   <si>
-    <t>Universal Pictures CampusU Marketing Representative</t>
-  </si>
-  <si>
     <t xml:space="preserve">MAISS, President of Marketing Association ('21-'22) </t>
   </si>
   <si>
@@ -1259,18 +1136,12 @@
     <t xml:space="preserve">Finance, Product Management </t>
   </si>
   <si>
-    <t>Product Development Intern at Billabong</t>
-  </si>
-  <si>
     <t>MUSA; Associate</t>
   </si>
   <si>
     <t>Hi! My name is Jake and I initiated in the fall of my freshman year with the Alpha Mu class. In my free time I enjoy surfing, playing tennis and listening to music. Ask me about my favorite comedians, or anything at recruitment!</t>
   </si>
   <si>
-    <t>Consulting Summer Scholar Intern at Deloitte</t>
-  </si>
-  <si>
     <t>ASUCI Media &amp; Technology Commission, Merage Specialty Masters Student Assistant, Product Association Fellowship</t>
   </si>
   <si>
@@ -1542,6 +1413,135 @@
   </si>
   <si>
     <t>Product Management, Marketing</t>
+  </si>
+  <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>Commit the Change, Product Association</t>
+  </si>
+  <si>
+    <t>Marketing, Product Management, Public Relations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campus Recreation, UC Irvine Club Volleyball, UUMP </t>
+  </si>
+  <si>
+    <t>Hi! My name is Maddie and I initiated the spring quarter of my second year with the Alpha Nu class. In my free time, you can find me at the ARC playing volleyball or watching tv/movies. Feel free to ask me about my favorite animal or my 150+ Spotify playlists at recruitment.</t>
+  </si>
+  <si>
+    <t>Health Informatics, Innovation and Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Information &amp; Computer Science</t>
+  </si>
+  <si>
+    <t>Consulting, Esports/Gaming, Product Management</t>
+  </si>
+  <si>
+    <t>180 Degrees Consulting, MUSA Representative</t>
+  </si>
+  <si>
+    <t>UCI ANTrepreneur Center, Mesa Court Housing, Sigma Chi, REA</t>
+  </si>
+  <si>
+    <t>Hello! My name is Aryan, and I initiated the spring quarter of my freshman year with the Alpha Nu class! In my free time, you will find me exploring nature, staying active at the gym, and playing soccer. A fun fact about me is that I stuck my finger in a blender when I was a kid. Ask me about Formula 1 or my passion for cars at recruitment, I look forward to meeting you!</t>
+  </si>
+  <si>
+    <t>Vice President of Technology @ MUSA</t>
+  </si>
+  <si>
+    <t>Consulting Summer Scholar Intern @ Deloitte</t>
+  </si>
+  <si>
+    <t>Project Manager @ Modulim</t>
+  </si>
+  <si>
+    <t>Marketing Intern @ UCI Athletics</t>
+  </si>
+  <si>
+    <t>UX Research Intern @ Zendesk</t>
+  </si>
+  <si>
+    <t>Marketing Intern @ KUCI 88.9 FM</t>
+  </si>
+  <si>
+    <t>Software Engineering Intern @ Duck Creek Technologies</t>
+  </si>
+  <si>
+    <t>UX Design Intern @ The Good</t>
+  </si>
+  <si>
+    <t>Risk and Financial Advisory Intern @ Deloitte</t>
+  </si>
+  <si>
+    <t>Private Equity Investment Intern @ Pathway Capital Management</t>
+  </si>
+  <si>
+    <t>Social Media Intern @ J.ING</t>
+  </si>
+  <si>
+    <t>Project Management Intern @ CBRE</t>
+  </si>
+  <si>
+    <t>CampusU Marketing Representative @ Universal Pictures</t>
+  </si>
+  <si>
+    <t>Venture Capital and Business Analytic Extern @ HP Tech Ventures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance/Business Operations Acquisition Intern @ NASA Jet Propulsion Laboratory </t>
+  </si>
+  <si>
+    <t>Business Strategy &amp; Marketing Intern @ Autodesk</t>
+  </si>
+  <si>
+    <t>Incoming Educator @ Lululemon</t>
+  </si>
+  <si>
+    <t>Product Development Intern @ Billabong</t>
+  </si>
+  <si>
+    <t>Partner @ California Crescent Fund</t>
+  </si>
+  <si>
+    <t>Finance Extern @ Apple; Client Group Intern @ Wellington</t>
+  </si>
+  <si>
+    <t>Private Equity Summer Analyst @ The Everstone Group</t>
+  </si>
+  <si>
+    <t>Intern @ Linda S. Congleton &amp; Associates</t>
+  </si>
+  <si>
+    <t>Change Management Operations Intern @ PayPal</t>
+  </si>
+  <si>
+    <t>Investment Banking Summer Analyst @ Deutsche Bank</t>
+  </si>
+  <si>
+    <t>Acquisition Analyst @ Next Wave Investors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer Research Consulting Intern @ Linda S. Congleton &amp; Associates </t>
+  </si>
+  <si>
+    <t>Accounting Project Associate @ First Foundation Bank</t>
+  </si>
+  <si>
+    <t>Portfolio Analyst Intern @ Wells Fargo Advisors</t>
+  </si>
+  <si>
+    <t>Finance Intern @ Facebook</t>
+  </si>
+  <si>
+    <t>Software Developer @ LinQuest</t>
+  </si>
+  <si>
+    <t>HR Intern @ Kaiser Permanente</t>
+  </si>
+  <si>
+    <t>Founder @ A Drop of Delight</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +1970,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1984,10 +1984,10 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="198" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
+      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2062,32 +2062,32 @@
         <v>44404.516250000001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>315</v>
+        <v>478</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>31</v>
@@ -2096,60 +2096,60 @@
         <v>67</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>344</v>
+        <v>319</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>345</v>
+        <v>320</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>347</v>
+        <v>213</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>348</v>
+        <v>477</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>349</v>
+        <v>473</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>350</v>
+        <v>322</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>352</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2163,7 +2163,7 @@
         <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -2181,13 +2181,13 @@
         <v>65</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>415</v>
+        <v>476</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>416</v>
+        <v>373</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>47</v>
@@ -2199,7 +2199,7 @@
         <v>79</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>417</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2207,13 +2207,13 @@
         <v>44404.857893518521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>91</v>
@@ -2225,43 +2225,43 @@
         <v>34</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>178</v>
+        <v>44</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>179</v>
+        <v>475</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -2273,89 +2273,89 @@
         <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>321</v>
+        <v>469</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>322</v>
+        <v>479</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>374</v>
+        <v>342</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>375</v>
+        <v>343</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>376</v>
+        <v>344</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>377</v>
+        <v>345</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>378</v>
+        <v>346</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>379</v>
+        <v>480</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>380</v>
+        <v>347</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>381</v>
+        <v>348</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>382</v>
+        <v>349</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>383</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>338</v>
+        <v>313</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>17</v>
@@ -2370,25 +2370,25 @@
         <v>65</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="M8" t="s">
         <v>32</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>343</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2396,47 +2396,47 @@
         <v>44404.653217592589</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>405</v>
+        <v>481</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2444,108 +2444,108 @@
         <v>44397.382604166669</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>393</v>
+        <v>464</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>316</v>
+        <v>482</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>299</v>
+        <v>465</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>394</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>365</v>
+        <v>333</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="E11" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>368</v>
+        <v>336</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>369</v>
+        <v>337</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>371</v>
+        <v>339</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>372</v>
+        <v>340</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>373</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>23</v>
@@ -2560,25 +2560,25 @@
         <v>65</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>247</v>
+        <v>483</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N12" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2586,13 +2586,13 @@
         <v>44396.99622685185</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>91</v>
@@ -2601,34 +2601,34 @@
         <v>23</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2636,13 +2636,13 @@
         <v>44397.802523148152</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>91</v>
@@ -2658,10 +2658,10 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>233</v>
+        <v>485</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>41</v>
@@ -2670,39 +2670,39 @@
         <v>57</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>31</v>
@@ -2714,57 +2714,60 @@
         <v>20</v>
       </c>
       <c r="N15" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I16" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="J16" s="2" t="s">
-        <v>255</v>
+        <v>471</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>31</v>
+        <v>486</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>262</v>
+        <v>472</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N16" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2772,16 +2775,16 @@
         <v>44398.992349537039</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>23</v>
@@ -2793,169 +2796,169 @@
         <v>35</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>408</v>
+        <v>487</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>409</v>
+        <v>368</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>306</v>
+        <v>488</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N18" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>354</v>
+        <v>325</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
       <c r="E19" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>360</v>
+        <v>466</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>361</v>
+        <v>467</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>362</v>
+        <v>331</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>363</v>
+        <v>332</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>364</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>92</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>396</v>
+        <v>489</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>397</v>
+        <v>361</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N20" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>398</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
@@ -2969,7 +2972,7 @@
         <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>16</v>
@@ -2990,10 +2993,10 @@
         <v>30</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>166</v>
+        <v>490</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>49</v>
@@ -3005,98 +3008,98 @@
         <v>80</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>311</v>
+        <v>491</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>57</v>
       </c>
       <c r="N22" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>410</v>
+        <v>369</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>412</v>
+        <v>492</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>413</v>
+        <v>371</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N23" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>414</v>
+        <v>372</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3110,7 +3113,7 @@
         <v>28</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
@@ -3129,10 +3132,10 @@
         <v>30</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>392</v>
+        <v>359</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>32</v>
@@ -3144,7 +3147,7 @@
         <v>81</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3152,13 +3155,13 @@
         <v>44396.99490740741</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>91</v>
@@ -3173,48 +3176,48 @@
         <v>51</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>420</v>
+        <v>377</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>300</v>
+        <v>493</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N25" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="P25" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>24</v>
@@ -3224,22 +3227,22 @@
         <v>92</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>402</v>
+        <v>494</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N26" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3253,7 +3256,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>16</v>
@@ -3268,16 +3271,16 @@
         <v>19</v>
       </c>
       <c r="I27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>20</v>
@@ -3289,7 +3292,7 @@
         <v>82</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3297,16 +3300,16 @@
         <v>44409.99291666667</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
@@ -3319,10 +3322,10 @@
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>310</v>
+        <v>496</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>31</v>
@@ -3331,13 +3334,13 @@
         <v>67</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3351,7 +3354,7 @@
         <v>74</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>16</v>
@@ -3366,16 +3369,16 @@
         <v>24</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>399</v>
+        <v>497</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>400</v>
+        <v>363</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>26</v>
@@ -3387,7 +3390,7 @@
         <v>83</v>
       </c>
       <c r="P29" s="11" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3401,7 +3404,7 @@
         <v>53</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>16</v>
@@ -3419,13 +3422,13 @@
         <v>54</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>149</v>
+        <v>498</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>45</v>
@@ -3437,7 +3440,7 @@
         <v>84</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3451,7 +3454,7 @@
         <v>76</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>16</v>
@@ -3467,13 +3470,13 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>203</v>
+        <v>499</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>57</v>
@@ -3485,7 +3488,7 @@
         <v>85</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3493,63 +3496,63 @@
         <v>44404.80846064815</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>224</v>
+        <v>500</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>40</v>
@@ -3561,13 +3564,13 @@
         <v>35</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>332</v>
+        <v>501</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>31</v>
@@ -3576,13 +3579,13 @@
         <v>47</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3596,7 +3599,7 @@
         <v>37</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>16</v>
@@ -3605,7 +3608,7 @@
         <v>23</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>35</v>
@@ -3615,10 +3618,10 @@
         <v>25</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>198</v>
+        <v>502</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>26</v>
@@ -3630,7 +3633,7 @@
         <v>86</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3659,28 +3662,28 @@
         <v>24</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>92</v>
       </c>
       <c r="K35" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N35" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="P35" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3688,13 +3691,13 @@
         <v>44397.036516203705</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>91</v>
@@ -3703,7 +3706,7 @@
         <v>40</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>43</v>
@@ -3713,7 +3716,7 @@
         <v>44</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>395</v>
+        <v>504</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>41</v>
@@ -3722,13 +3725,13 @@
         <v>26</v>
       </c>
       <c r="N36" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P36" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3736,22 +3739,22 @@
         <v>44411.776064814818</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>24</v>
@@ -3761,69 +3764,69 @@
         <v>56</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>401</v>
+        <v>505</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>41</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>384</v>
+        <v>351</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>385</v>
+        <v>352</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>386</v>
+        <v>353</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>387</v>
+        <v>354</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>418</v>
+        <v>375</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>388</v>
+        <v>355</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>389</v>
+        <v>356</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>390</v>
+        <v>357</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>391</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3831,13 +3834,13 @@
         <v>44405.648368055554</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>91</v>
@@ -3846,34 +3849,34 @@
         <v>40</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>189</v>
+        <v>506</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3881,13 +3884,13 @@
         <v>44396.946180555555</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>91</v>
@@ -3899,225 +3902,225 @@
         <v>38</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2" t="s">
-        <v>421</v>
+        <v>378</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>422</v>
+        <v>379</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>423</v>
+        <v>380</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>92</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>466</v>
+        <v>423</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>428</v>
+        <v>385</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N41" t="s">
-        <v>429</v>
+        <v>386</v>
       </c>
       <c r="O41" s="13" t="s">
-        <v>430</v>
+        <v>387</v>
       </c>
       <c r="P41" s="14" t="s">
-        <v>431</v>
+        <v>388</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="14" t="s">
-        <v>432</v>
+        <v>389</v>
       </c>
       <c r="C42" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>436</v>
+        <v>393</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>440</v>
+        <v>397</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>24</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>439</v>
+        <v>396</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>438</v>
+        <v>395</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>437</v>
+        <v>394</v>
       </c>
       <c r="M42" s="12" t="s">
         <v>26</v>
       </c>
       <c r="N42" t="s">
-        <v>435</v>
+        <v>392</v>
       </c>
       <c r="O42" s="15" t="s">
-        <v>434</v>
+        <v>391</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>433</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>441</v>
+        <v>398</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>442</v>
+        <v>399</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>443</v>
+        <v>400</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>444</v>
+        <v>401</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>24</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>445</v>
+        <v>402</v>
       </c>
       <c r="K43" s="12" t="s">
         <v>31</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>446</v>
+        <v>403</v>
       </c>
       <c r="M43" t="s">
         <v>32</v>
       </c>
       <c r="N43" t="s">
-        <v>447</v>
+        <v>404</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>448</v>
+        <v>405</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
-        <v>450</v>
+        <v>407</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>451</v>
+        <v>408</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>455</v>
+        <v>412</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>464</v>
+        <v>421</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>452</v>
+        <v>409</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>453</v>
+        <v>410</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>454</v>
+        <v>411</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>460</v>
+        <v>417</v>
       </c>
       <c r="L44" s="14" t="s">
-        <v>459</v>
+        <v>416</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>45</v>
       </c>
       <c r="N44" t="s">
-        <v>456</v>
+        <v>413</v>
       </c>
       <c r="O44" s="13" t="s">
-        <v>457</v>
+        <v>414</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="14" t="s">
-        <v>461</v>
+        <v>418</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>463</v>
+        <v>420</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>48</v>
@@ -4126,51 +4129,51 @@
         <v>24</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>465</v>
+        <v>422</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>466</v>
+        <v>423</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>428</v>
+        <v>385</v>
       </c>
       <c r="M45" s="12" t="s">
         <v>57</v>
       </c>
       <c r="N45" t="s">
-        <v>469</v>
+        <v>426</v>
       </c>
       <c r="O45" s="17" t="s">
-        <v>468</v>
+        <v>425</v>
       </c>
       <c r="P45" s="14" t="s">
-        <v>467</v>
+        <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
-        <v>470</v>
+        <v>427</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>471</v>
+        <v>428</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>477</v>
+        <v>434</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>472</v>
+        <v>429</v>
       </c>
       <c r="H46" s="12" t="s">
         <v>35</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>30</v>
@@ -4179,127 +4182,127 @@
         <v>31</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>473</v>
+        <v>430</v>
       </c>
       <c r="M46" s="12" t="s">
         <v>49</v>
       </c>
       <c r="N46" t="s">
-        <v>476</v>
+        <v>433</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>475</v>
+        <v>432</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>474</v>
+        <v>431</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>478</v>
+        <v>435</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>480</v>
+        <v>437</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>481</v>
+        <v>438</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>35</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>482</v>
+        <v>439</v>
       </c>
       <c r="K47" s="12" t="s">
         <v>31</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="M47" s="12" t="s">
         <v>67</v>
       </c>
       <c r="N47" t="s">
-        <v>486</v>
+        <v>443</v>
       </c>
       <c r="O47" s="13" t="s">
-        <v>485</v>
+        <v>442</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>484</v>
+        <v>441</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
-        <v>487</v>
+        <v>444</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>488</v>
+        <v>445</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>489</v>
+        <v>446</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>490</v>
+        <v>447</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>493</v>
+        <v>450</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>494</v>
+        <v>451</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>26</v>
       </c>
       <c r="N48" t="s">
-        <v>497</v>
+        <v>454</v>
       </c>
       <c r="O48" s="13" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>495</v>
+        <v>452</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="12" t="s">
-        <v>498</v>
+        <v>455</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>503</v>
+        <v>460</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>504</v>
+        <v>461</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>24</v>
@@ -4308,25 +4311,25 @@
         <v>65</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>506</v>
+        <v>463</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>502</v>
+        <v>459</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>501</v>
+        <v>458</v>
       </c>
       <c r="M49" s="12" t="s">
         <v>32</v>
       </c>
       <c r="N49" t="s">
-        <v>497</v>
+        <v>454</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>499</v>
+        <v>456</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>500</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>